<commit_message>
Added replication master dofile
Created 1 dofile to ensure replication of all results.
</commit_message>
<xml_diff>
--- a/5.figures/Path_for_reproduction.xlsx
+++ b/5.figures/Path_for_reproduction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB378870\GitHub\S2S_RTM\5.figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF73609-75F1-4C46-A50D-D46014A61377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4409C6E-996E-4174-AF22-A33A1D572ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{0A9F2F42-FA68-4FF3-B0C6-4A7D73B24E79}"/>
+    <workbookView xWindow="9518" yWindow="0" windowWidth="9765" windowHeight="11363" xr2:uid="{0A9F2F42-FA68-4FF3-B0C6-4A7D73B24E79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -559,18 +559,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0675C2B6-E9AA-4FB8-8B4D-DE6CB5522995}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="87.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -587,7 +587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -604,7 +604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -621,7 +621,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -638,7 +638,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -655,7 +655,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -672,7 +672,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -689,7 +689,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -706,7 +706,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -723,7 +723,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -740,7 +740,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -757,7 +757,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -774,7 +774,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -791,7 +791,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -808,7 +808,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -825,7 +825,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -842,7 +842,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -859,12 +859,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>1</v>
       </c>
@@ -881,7 +881,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>2</v>
       </c>
@@ -898,7 +898,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>3</v>
       </c>
@@ -915,7 +915,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>4</v>
       </c>
@@ -932,7 +932,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>5</v>
       </c>

</xml_diff>